<commit_message>
add example values to mandatory ENA templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/ENA/ENA_-_Gene_promoter_annotated_sequence.xlsx
+++ b/templates/dataplant/ENA/ENA_-_Gene_promoter_annotated_sequence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Description</t>
@@ -249,6 +249,27 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Zea mays</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_4577</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>ZmAbh1</t>
   </si>
 </sst>
 </file>
@@ -977,16 +998,16 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
         <v>78</v>
@@ -995,7 +1016,7 @@
         <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
         <v>78</v>
@@ -1004,7 +1025,7 @@
         <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="L2" t="s">
         <v>78</v>
@@ -1013,7 +1034,7 @@
         <v>78</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
         <v>78</v>
@@ -1022,7 +1043,7 @@
         <v>78</v>
       </c>
       <c r="Q2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="R2" t="s">
         <v>78</v>
@@ -1031,7 +1052,7 @@
         <v>78</v>
       </c>
       <c r="T2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="U2" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
update TSRs in ENA templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/ENA/ENA_-_Gene_promoter_annotated_sequence.xlsx
+++ b/templates/dataplant/ENA/ENA_-_Gene_promoter_annotated_sequence.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="87">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Description</t>
@@ -170,16 +170,16 @@
     <t>Author Roles Term Source REF</t>
   </si>
   <si>
-    <t>Input [Raw Data File]</t>
-  </si>
-  <si>
-    <t>Characteristic [ORGANISM_NAME]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C179773)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C179773)</t>
+    <t>Input [Data]</t>
+  </si>
+  <si>
+    <t>Characteristic [organism]</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0100026)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0100026)</t>
   </si>
   <si>
     <t>Characteristic [BI_PROM]</t>
@@ -245,7 +245,7 @@
     <t>Term Accession Number (SIO:010016)</t>
   </si>
   <si>
-    <t>Output [Derived Data File]</t>
+    <t>Output [Data]</t>
   </si>
   <si>
     <t/>
@@ -260,7 +260,10 @@
     <t>http://purl.obolibrary.org/obo/NCBITaxon_4577</t>
   </si>
   <si>
-    <t>no</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/NCIT:C49487</t>
   </si>
   <si>
     <t>1</t>
@@ -355,10 +358,10 @@
     <filterColumn colId="25" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="26">
-    <tableColumn id="1" name="Input [Raw Data File]" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Characteristic [ORGANISM_NAME]" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Term Source REF (NCIT:C179773)" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Term Accession Number (NCIT:C179773)" totalsRowFunction="none"/>
+    <tableColumn id="1" name="Input [Data]" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Characteristic [organism]" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Term Source REF (OBI:0100026)" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Term Accession Number (OBI:0100026)" totalsRowFunction="none"/>
     <tableColumn id="5" name="Characteristic [BI_PROM]" totalsRowFunction="none"/>
     <tableColumn id="6" name="Term Source REF (SO:0000568)" totalsRowFunction="none"/>
     <tableColumn id="7" name="Term Accession Number (SO:0000568)" totalsRowFunction="none"/>
@@ -380,7 +383,7 @@
     <tableColumn id="23" name="Characteristic [SEQUENCE]" totalsRowFunction="none"/>
     <tableColumn id="24" name="Term Source REF (SIO:010016)" totalsRowFunction="none"/>
     <tableColumn id="25" name="Term Accession Number (SIO:010016)" totalsRowFunction="none"/>
-    <tableColumn id="26" name="Output [Derived Data File]" totalsRowFunction="none"/>
+    <tableColumn id="26" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,13 +1013,13 @@
         <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
         <v>78</v>
@@ -1025,7 +1028,7 @@
         <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
         <v>78</v>
@@ -1037,22 +1040,22 @@
         <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Q2" t="s">
         <v>82</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="U2" t="s">
         <v>78</v>

</xml_diff>